<commit_message>
terminer test app user
</commit_message>
<xml_diff>
--- a/managment_tournoi_backend/src/main/resources/xlsx/membersUpload.xlsx
+++ b/managment_tournoi_backend/src/main/resources/xlsx/membersUpload.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,60 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">first name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Url Pic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mohammed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moussafia</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">m,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">moussafia@gmail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">,com</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">kjgdskljgk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">htt:hfjdhsjk</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t xml:space="preserve">First name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Url Intranet</t>
   </si>
 </sst>
 </file>
@@ -83,11 +44,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+  <fonts count="7">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -105,18 +67,40 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,8 +137,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,52 +175,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="moussafia@gmail"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>